<commit_message>
zip to lat lon et model
</commit_message>
<xml_diff>
--- a/EXAM/Model_comparison.xlsx
+++ b/EXAM/Model_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mingjiexing/Desktop/23 Summer/Copenhagen/SODAS2023_GithubDesktop/EXAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C500E88-7B89-924F-860A-5F61803D1110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF7F16A-7493-B147-A03A-02F9EAFAF175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16540" xr2:uid="{2F864CB2-3578-2640-810C-E0985A81B903}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="B3:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +607,9 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>2710335.5680292002</v>
+      </c>
       <c r="D8" s="2">
         <v>0.24503146813842799</v>
       </c>
@@ -639,7 +641,9 @@
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>2995998.4088369301</v>
+      </c>
       <c r="D11" s="2">
         <v>7.7501055527137305E-2</v>
       </c>

</xml_diff>